<commit_message>
feat: update lecturer template
</commit_message>
<xml_diff>
--- a/public/template/lecturer.xlsx
+++ b/public/template/lecturer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aonro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puntf\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3521C8A-1B44-4F47-BB52-1830BAA99E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B83C04A-9651-4206-AAC5-82438B18D1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{89ADDBAD-9FE3-4804-AC9F-F22C98C6D307}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89ADDBAD-9FE3-4804-AC9F-F22C98C6D307}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>firstname</t>
   </si>
   <si>
     <t>lastname</t>
@@ -52,6 +46,9 @@
   <si>
     <t>role</t>
   </si>
+  <si>
+    <t>_firstname</t>
+  </si>
 </sst>
 </file>
 
@@ -61,7 +58,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -106,13 +103,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A49154BF-37C5-4A4E-916E-B4765B3D0694}" name="Table1" displayName="Table1" ref="A1:E2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:E2" xr:uid="{A49154BF-37C5-4A4E-916E-B4765B3D0694}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4EE62F39-FE89-4E59-9D04-EEC577CCFA6F}" name="name"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A49154BF-37C5-4A4E-916E-B4765B3D0694}" name="Table1" displayName="Table1" ref="A1:D2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{A49154BF-37C5-4A4E-916E-B4765B3D0694}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{4EE62F39-FE89-4E59-9D04-EEC577CCFA6F}" name="_firstname"/>
+    <tableColumn id="6" xr3:uid="{C35E9453-8B3A-420A-A33C-4871245790F6}" name="lastname"/>
     <tableColumn id="2" xr3:uid="{F7C1328F-7C9C-4578-9968-CCF66F7C1903}" name="email"/>
-    <tableColumn id="3" xr3:uid="{A8763484-E27A-4690-B8DB-4F588471455F}" name="firstname"/>
-    <tableColumn id="4" xr3:uid="{3874DAD4-3050-4B07-86A5-4918FFD39B1A}" name="lastname"/>
     <tableColumn id="5" xr3:uid="{D83482DB-546A-47EB-8AB4-F46AC60BA122}" name="role"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -416,37 +412,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE034EC-E592-48DB-9173-CD90C74093B9}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="8.81640625" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="14.25" customWidth="1"/>
+    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{2B5E58E1-A165-4588-8AC2-7170C1862801}">
+      <formula1>"lecturer, tabee manager, head of curriculum, moderator"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>